<commit_message>
Project Tutorial 1 - Introduction to Decision Tables is saved. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Tutorial 1 - Introduction to Decision Tables/Tutorial1 - Intro to Decision Tables.xlsx
+++ b/DESIGN/rules/Tutorial 1 - Introduction to Decision Tables/Tutorial1 - Intro to Decision Tables.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\openl-demo-app-5.23.3\apache-tomcat-9.0.30\openl-demo\user-workspace\DEFAULT\Tutorial 1 - Introduction to Decision Tables\"/>
     </mc:Choice>
@@ -403,20 +403,6 @@
             <charset val="204"/>
           </rPr>
           <t>Vertical condition values</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D69" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-            <charset val="204"/>
-          </rPr>
-          <t xml:space="preserve">The height of the first column title cell = Number of horizontal conditions </t>
         </r>
       </text>
     </comment>
@@ -3101,9 +3087,9 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="9" width="9.109375" style="3" collapsed="1"/>
-    <col min="10" max="10" width="19.109375" style="3" customWidth="1" collapsed="1"/>
-    <col min="11" max="16384" width="9.109375" style="3" collapsed="1"/>
+    <col min="1" max="9" style="3" width="9.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="3" width="19.109375" collapsed="true"/>
+    <col min="11" max="16384" style="3" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:11" ht="22.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -3613,13 +3599,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.109375" style="1" collapsed="1"/>
-    <col min="4" max="4" width="19" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.88671875" style="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="42.44140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.109375" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="10.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="8.109375" collapsed="true"/>
+    <col min="3" max="3" style="1" width="9.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="19.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="1" width="19.88671875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="42.44140625" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" s="3" customFormat="1" ht="13.8" x14ac:dyDescent="0.3"/>
@@ -4810,14 +4796,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="8" collapsed="1"/>
-    <col min="3" max="3" width="7.6640625" style="8" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="55.44140625" style="8" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="16.44140625" style="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.5546875" style="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="14.33203125" style="8" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="16.109375" style="8" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.109375" style="8" collapsed="1"/>
+    <col min="1" max="2" style="8" width="9.109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="8" width="7.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="8" width="55.44140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="8" width="16.44140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="8" width="12.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" style="8" width="14.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="8" width="16.109375" collapsed="true"/>
+    <col min="9" max="16384" style="8" width="9.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3"/>
@@ -5539,127 +5525,36 @@
     <row r="68" spans="2:9" s="11" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B68" s="12"/>
       <c r="C68" s="12"/>
-      <c r="D68" s="79" t="s">
-        <v>117</v>
-      </c>
-      <c r="E68" s="79"/>
-      <c r="F68" s="79"/>
-      <c r="G68" s="79"/>
-      <c r="H68" s="79"/>
       <c r="I68" s="12"/>
     </row>
     <row r="69" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B69" s="12"/>
       <c r="C69" s="12"/>
-      <c r="D69" s="89" t="s">
-        <v>111</v>
-      </c>
-      <c r="E69" s="94" t="s">
-        <v>42</v>
-      </c>
-      <c r="F69" s="94"/>
-      <c r="G69" s="94" t="s">
-        <v>56</v>
-      </c>
-      <c r="H69" s="94"/>
       <c r="I69" s="12"/>
     </row>
     <row r="70" spans="2:9" s="11" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B70" s="12"/>
       <c r="C70" s="12"/>
-      <c r="D70" s="89"/>
-      <c r="E70" s="52" t="s">
-        <v>57</v>
-      </c>
-      <c r="F70" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="G70" s="58" t="s">
-        <v>60</v>
-      </c>
-      <c r="H70" s="52" t="s">
-        <v>61</v>
-      </c>
       <c r="I70" s="12"/>
     </row>
     <row r="71" spans="2:9" s="11" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B71" s="12"/>
       <c r="C71" s="12"/>
-      <c r="D71" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="E71" s="53">
-        <v>55150</v>
-      </c>
-      <c r="F71" s="56">
-        <v>47350</v>
-      </c>
-      <c r="G71" s="56">
-        <v>105630</v>
-      </c>
-      <c r="H71" s="50">
-        <v>91030</v>
-      </c>
       <c r="I71" s="12"/>
     </row>
     <row r="72" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B72" s="12"/>
       <c r="C72" s="12"/>
-      <c r="D72" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E72" s="30">
-        <v>57150</v>
-      </c>
-      <c r="F72" s="26">
-        <v>49350</v>
-      </c>
-      <c r="G72" s="26">
-        <v>107630</v>
-      </c>
-      <c r="H72" s="26">
-        <v>93220</v>
-      </c>
       <c r="I72" s="12"/>
     </row>
     <row r="73" spans="2:9" s="11" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="B73" s="12"/>
       <c r="C73" s="12"/>
-      <c r="D73" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E73" s="32">
-        <v>64400</v>
-      </c>
-      <c r="F73" s="33">
-        <v>57150</v>
-      </c>
-      <c r="G73" s="33">
-        <v>125600</v>
-      </c>
-      <c r="H73" s="33">
-        <v>110030</v>
-      </c>
       <c r="I73" s="12"/>
     </row>
     <row r="74" spans="2:9" s="11" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B74" s="12"/>
       <c r="C74" s="12"/>
-      <c r="D74" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E74" s="54">
-        <v>90400</v>
-      </c>
-      <c r="F74" s="57">
-        <v>83500</v>
-      </c>
-      <c r="G74" s="57">
-        <v>145500</v>
-      </c>
-      <c r="H74" s="55">
-        <v>130500</v>
-      </c>
       <c r="I74" s="12"/>
     </row>
     <row r="75" spans="2:9" s="11" customFormat="1" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
@@ -5739,8 +5634,6 @@
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="C60:F60"/>
     <mergeCell ref="C63:F65"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="D68:H68"/>
     <mergeCell ref="E50:F50"/>
     <mergeCell ref="C53:F54"/>
     <mergeCell ref="C8:F9"/>
@@ -5750,8 +5643,6 @@
     <mergeCell ref="C37:F37"/>
     <mergeCell ref="C40:F43"/>
     <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="G69:H69"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D79" location="_st3" tooltip="Step3. Examples of Decision Tables" display="Step 3." xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -5773,16 +5664,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="21.88671875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.5546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="9.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="21.88671875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.44140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="14.5546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>